<commit_message>
add 2 instructions(beq bne)
</commit_message>
<xml_diff>
--- a/add.xlsx
+++ b/add.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18060" windowHeight="9684" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18060" windowHeight="9684" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="add" sheetId="1" r:id="rId1"/>
@@ -17,8 +17,11 @@
     <sheet name="sw" sheetId="3" r:id="rId3"/>
     <sheet name="j" sheetId="6" r:id="rId4"/>
     <sheet name="jal" sheetId="7" r:id="rId5"/>
-    <sheet name="mux" sheetId="4" r:id="rId6"/>
-    <sheet name="cu" sheetId="5" r:id="rId7"/>
+    <sheet name="beq" sheetId="9" r:id="rId6"/>
+    <sheet name="bne" sheetId="8" r:id="rId7"/>
+    <sheet name="mux" sheetId="4" r:id="rId8"/>
+    <sheet name="cu" sheetId="5" r:id="rId9"/>
+    <sheet name="Alu" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="214">
   <si>
     <t>阶段</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -660,9 +663,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>lw|sw</t>
-  </si>
-  <si>
     <t>读取base所指向的寄存器的值，加上offset左移两位后的值，读取求和得到内存的位置，把rt复制给它</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -690,10 +690,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>add|lw|sw|j|jal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>p2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -702,14 +698,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>gr.writedata</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>gr.writeregister</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>!</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -722,10 +710,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>lw|sw</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>p2</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -735,6 +719,9 @@
   </si>
   <si>
     <t>EX</t>
+  </si>
+  <si>
+    <t>EX</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -755,6 +742,129 @@
   </si>
   <si>
     <t>jal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC.WriteCond</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC.out</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shift←2.out</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC.IN</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>lw|sw|beq|bne</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>6'b010001</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>beq|bne</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>beq|bne</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6'b100001</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>p1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>p2/p1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lw|sw/beq|bne</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>操作名</t>
+  </si>
+  <si>
+    <t>功能码</t>
+  </si>
+  <si>
+    <t>加</t>
+  </si>
+  <si>
+    <t>减</t>
+  </si>
+  <si>
+    <t>与</t>
+  </si>
+  <si>
+    <t>或</t>
+  </si>
+  <si>
+    <t>或非</t>
+  </si>
+  <si>
+    <t>与非</t>
+  </si>
+  <si>
+    <t>无符号小于</t>
+  </si>
+  <si>
+    <t>有符号小于</t>
+  </si>
+  <si>
+    <t>异或</t>
+  </si>
+  <si>
+    <t>不等</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>相等</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000010</t>
+  </si>
+  <si>
+    <t>000100</t>
+  </si>
+  <si>
+    <t>001000</t>
+  </si>
+  <si>
+    <t>010000</t>
+  </si>
+  <si>
+    <t>100000</t>
+  </si>
+  <si>
+    <t>000011</t>
+  </si>
+  <si>
+    <t>000101</t>
+  </si>
+  <si>
+    <t>001001</t>
+  </si>
+  <si>
+    <t>010001</t>
+  </si>
+  <si>
+    <t>100001</t>
+  </si>
+  <si>
+    <t>EX</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -762,7 +872,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -785,6 +895,19 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10.5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -794,10 +917,73 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -808,7 +994,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -816,6 +1002,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1133,8 +1337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:E29"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1331,7 +1535,7 @@
         <v>30</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
@@ -1525,6 +1729,122 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="13.77734375" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" thickBot="1">
+      <c r="A1" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15" thickBot="1">
+      <c r="A2" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" thickBot="1">
+      <c r="A3" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15" thickBot="1">
+      <c r="A4" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15" thickBot="1">
+      <c r="A5" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15" thickBot="1">
+      <c r="A6" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15" thickBot="1">
+      <c r="A7" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="29.4" thickBot="1">
+      <c r="A8" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="29.4" thickBot="1">
+      <c r="A9" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15" thickBot="1">
+      <c r="A10" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15" thickBot="1">
+      <c r="A11" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="B12" s="9">
+        <v>100011</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1533,7 +1853,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A11" sqref="A11:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1918,7 +2238,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -2256,7 +2576,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2376,7 +2696,7 @@
         <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>87</v>
@@ -2389,10 +2709,10 @@
         <v>32</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -2498,7 +2818,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2618,7 +2938,7 @@
         <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>87</v>
@@ -2628,13 +2948,13 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -2644,10 +2964,10 @@
         <v>109</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>168</v>
+        <v>52</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -2660,7 +2980,7 @@
         <v>31</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>169</v>
+        <v>50</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -2749,10 +3069,800 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E37"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="23.77734375" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E37"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="23.77734375" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2828,7 +3938,7 @@
         <v>122</v>
       </c>
       <c r="E4" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2879,7 +3989,7 @@
         <v>120</v>
       </c>
       <c r="E7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2887,13 +3997,13 @@
         <v>87</v>
       </c>
       <c r="B8" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>82</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -2902,12 +4012,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2938,7 +4048,7 @@
         <v>117</v>
       </c>
       <c r="G1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H1" t="s">
         <v>155</v>
@@ -2981,10 +4091,10 @@
         <v>150</v>
       </c>
       <c r="F3" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="G3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -3004,10 +4114,10 @@
         <v>149</v>
       </c>
       <c r="F4" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="G4" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -3015,10 +4125,10 @@
         <v>140</v>
       </c>
       <c r="B5" t="s">
-        <v>123</v>
+        <v>187</v>
       </c>
       <c r="C5" t="s">
-        <v>146</v>
+        <v>184</v>
       </c>
       <c r="D5" t="s">
         <v>148</v>
@@ -3047,33 +4157,27 @@
         <v>116</v>
       </c>
       <c r="H6" t="s">
-        <v>148</v>
+        <v>188</v>
       </c>
       <c r="I6" t="s">
-        <v>157</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>142</v>
       </c>
-      <c r="B7" t="s">
-        <v>123</v>
-      </c>
-      <c r="C7" t="s">
-        <v>165</v>
-      </c>
       <c r="D7" t="s">
-        <v>116</v>
+        <v>148</v>
       </c>
       <c r="E7" t="s">
-        <v>134</v>
+        <v>185</v>
       </c>
       <c r="F7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H7" t="s">
         <v>134</v>
@@ -3081,19 +4185,19 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B8" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E8" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add 3 instructions(slt jr jalr)
</commit_message>
<xml_diff>
--- a/add.xlsx
+++ b/add.xlsx
@@ -9,19 +9,22 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18060" windowHeight="9684" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18060" windowHeight="9684" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="add" sheetId="1" r:id="rId1"/>
     <sheet name="lw" sheetId="2" r:id="rId2"/>
     <sheet name="sw" sheetId="3" r:id="rId3"/>
     <sheet name="j" sheetId="6" r:id="rId4"/>
-    <sheet name="jal" sheetId="7" r:id="rId5"/>
-    <sheet name="beq" sheetId="9" r:id="rId6"/>
-    <sheet name="bne" sheetId="8" r:id="rId7"/>
-    <sheet name="mux" sheetId="4" r:id="rId8"/>
-    <sheet name="cu" sheetId="5" r:id="rId9"/>
-    <sheet name="Alu" sheetId="10" r:id="rId10"/>
+    <sheet name="jr" sheetId="12" r:id="rId5"/>
+    <sheet name="jal" sheetId="7" r:id="rId6"/>
+    <sheet name="jalr" sheetId="13" r:id="rId7"/>
+    <sheet name="beq" sheetId="9" r:id="rId8"/>
+    <sheet name="bne" sheetId="8" r:id="rId9"/>
+    <sheet name="slt" sheetId="11" r:id="rId10"/>
+    <sheet name="mux" sheetId="4" r:id="rId11"/>
+    <sheet name="cu" sheetId="5" r:id="rId12"/>
+    <sheet name="Alu" sheetId="10" r:id="rId13"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="228">
   <si>
     <t>阶段</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -725,10 +728,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PC.NEXT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>p4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -865,6 +864,66 @@
   </si>
   <si>
     <t>EX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALUOUT.out</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">0^31 + ALUOUT.out </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GPR.RREG1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>返回A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>返回B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>101001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6'b100101</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>6'b100101</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MDR.IN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mdrINCtrl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DMEM.out</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC.next</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MDR.in</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MDR.IN</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1337,8 +1396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:E29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:C20"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C12" sqref="A12:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1734,10 +1793,673 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="23.77734375" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="11.21875" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="23.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E7" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" t="s">
+        <v>167</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>222</v>
+      </c>
+      <c r="B9" t="s">
+        <v>223</v>
+      </c>
+      <c r="C9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D9" t="s">
+        <v>225</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="2" width="10.77734375" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G1" t="s">
+        <v>162</v>
+      </c>
+      <c r="H1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E3" t="s">
+        <v>150</v>
+      </c>
+      <c r="F3" t="s">
+        <v>173</v>
+      </c>
+      <c r="G3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D4" t="s">
+        <v>153</v>
+      </c>
+      <c r="E4" t="s">
+        <v>149</v>
+      </c>
+      <c r="F4" t="s">
+        <v>175</v>
+      </c>
+      <c r="G4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D5" t="s">
+        <v>148</v>
+      </c>
+      <c r="E5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C6" t="s">
+        <v>150</v>
+      </c>
+      <c r="D6" t="s">
+        <v>123</v>
+      </c>
+      <c r="E6" t="s">
+        <v>146</v>
+      </c>
+      <c r="F6" t="s">
+        <v>116</v>
+      </c>
+      <c r="H6" t="s">
+        <v>187</v>
+      </c>
+      <c r="I6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>142</v>
+      </c>
+      <c r="D7" t="s">
+        <v>148</v>
+      </c>
+      <c r="E7" t="s">
+        <v>184</v>
+      </c>
+      <c r="F7" t="s">
+        <v>164</v>
+      </c>
+      <c r="G7" t="s">
+        <v>163</v>
+      </c>
+      <c r="H7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1748,98 +2470,114 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1">
       <c r="A1" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>190</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" thickBot="1">
       <c r="A2" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" thickBot="1">
       <c r="A3" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" thickBot="1">
       <c r="A4" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" thickBot="1">
       <c r="A5" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" thickBot="1">
       <c r="A6" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" thickBot="1">
       <c r="A7" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="29.4" thickBot="1">
       <c r="A8" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="29.4" thickBot="1">
       <c r="A9" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15" thickBot="1">
       <c r="A10" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15" thickBot="1">
       <c r="A11" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B12" s="9">
         <v>100011</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -2815,10 +3553,308 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="16.109375" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A13" sqref="A13:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2948,26 +3984,26 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>172</v>
+        <v>81</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>160</v>
+        <v>226</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
-        <v>109</v>
+        <v>172</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>52</v>
+        <v>160</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -2976,19 +4012,25 @@
       <c r="A13" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B13" s="1">
-        <v>31</v>
+      <c r="B13" s="1" t="s">
+        <v>227</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B14" s="1">
+        <v>31</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
@@ -3067,12 +4109,333 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="16.109375" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="C26" sqref="A26:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3244,7 +4607,7 @@
         <v>81</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>124</v>
@@ -3257,7 +4620,7 @@
         <v>81</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>36</v>
@@ -3367,7 +4730,7 @@
         <v>32</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>38</v>
@@ -3383,20 +4746,20 @@
         <v>39</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="C26" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -3462,12 +4825,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3639,7 +5002,7 @@
         <v>81</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>124</v>
@@ -3652,7 +5015,7 @@
         <v>81</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>36</v>
@@ -3766,7 +5129,7 @@
         <v>32</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>38</v>
@@ -3780,7 +5143,7 @@
         <v>39</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -3788,10 +5151,10 @@
         <v>171</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>40</v>
+        <v>213</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -3855,354 +5218,4 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="11.21875" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" customWidth="1"/>
-    <col min="5" max="5" width="23.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>110</v>
-      </c>
-      <c r="B3" t="s">
-        <v>138</v>
-      </c>
-      <c r="C3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E3">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>121</v>
-      </c>
-      <c r="B4" t="s">
-        <v>139</v>
-      </c>
-      <c r="C4" t="s">
-        <v>120</v>
-      </c>
-      <c r="D4" t="s">
-        <v>122</v>
-      </c>
-      <c r="E4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B5" t="s">
-        <v>140</v>
-      </c>
-      <c r="C5" t="s">
-        <v>119</v>
-      </c>
-      <c r="D5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>126</v>
-      </c>
-      <c r="B6" t="s">
-        <v>141</v>
-      </c>
-      <c r="C6" t="s">
-        <v>128</v>
-      </c>
-      <c r="D6" t="s">
-        <v>129</v>
-      </c>
-      <c r="E6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F6" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>132</v>
-      </c>
-      <c r="B7" t="s">
-        <v>142</v>
-      </c>
-      <c r="C7" t="s">
-        <v>133</v>
-      </c>
-      <c r="D7" t="s">
-        <v>120</v>
-      </c>
-      <c r="E7" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B8" t="s">
-        <v>167</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="2" width="10.77734375" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E1" t="s">
-        <v>152</v>
-      </c>
-      <c r="F1" t="s">
-        <v>117</v>
-      </c>
-      <c r="G1" t="s">
-        <v>162</v>
-      </c>
-      <c r="H1" t="s">
-        <v>155</v>
-      </c>
-      <c r="I1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B2" t="s">
-        <v>145</v>
-      </c>
-      <c r="C2" t="s">
-        <v>146</v>
-      </c>
-      <c r="D2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>138</v>
-      </c>
-      <c r="B3" t="s">
-        <v>147</v>
-      </c>
-      <c r="C3" t="s">
-        <v>149</v>
-      </c>
-      <c r="D3" t="s">
-        <v>147</v>
-      </c>
-      <c r="E3" t="s">
-        <v>150</v>
-      </c>
-      <c r="F3" t="s">
-        <v>174</v>
-      </c>
-      <c r="G3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
-        <v>139</v>
-      </c>
-      <c r="B4" t="s">
-        <v>147</v>
-      </c>
-      <c r="C4" t="s">
-        <v>150</v>
-      </c>
-      <c r="D4" t="s">
-        <v>153</v>
-      </c>
-      <c r="E4" t="s">
-        <v>149</v>
-      </c>
-      <c r="F4" t="s">
-        <v>176</v>
-      </c>
-      <c r="G4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
-        <v>140</v>
-      </c>
-      <c r="B5" t="s">
-        <v>187</v>
-      </c>
-      <c r="C5" t="s">
-        <v>184</v>
-      </c>
-      <c r="D5" t="s">
-        <v>148</v>
-      </c>
-      <c r="E5" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" t="s">
-        <v>141</v>
-      </c>
-      <c r="B6" t="s">
-        <v>148</v>
-      </c>
-      <c r="C6" t="s">
-        <v>150</v>
-      </c>
-      <c r="D6" t="s">
-        <v>123</v>
-      </c>
-      <c r="E6" t="s">
-        <v>146</v>
-      </c>
-      <c r="F6" t="s">
-        <v>116</v>
-      </c>
-      <c r="H6" t="s">
-        <v>188</v>
-      </c>
-      <c r="I6" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
-        <v>142</v>
-      </c>
-      <c r="D7" t="s">
-        <v>148</v>
-      </c>
-      <c r="E7" t="s">
-        <v>185</v>
-      </c>
-      <c r="F7" t="s">
-        <v>164</v>
-      </c>
-      <c r="G7" t="s">
-        <v>163</v>
-      </c>
-      <c r="H7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" t="s">
-        <v>167</v>
-      </c>
-      <c r="B8" t="s">
-        <v>168</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="E8" t="s">
-        <v>170</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
add lui & shifts(sra,srav,srl,srlv,sll,sllv)
</commit_message>
<xml_diff>
--- a/add.xlsx
+++ b/add.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18060" windowHeight="9684" firstSheet="2" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18060" windowHeight="9684" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="add" sheetId="1" r:id="rId1"/>
@@ -22,9 +22,10 @@
     <sheet name="branch" sheetId="9" r:id="rId8"/>
     <sheet name="simpcR" sheetId="14" r:id="rId9"/>
     <sheet name="simpcI" sheetId="18" r:id="rId10"/>
-    <sheet name="mux" sheetId="4" r:id="rId11"/>
-    <sheet name="cu" sheetId="5" r:id="rId12"/>
-    <sheet name="Alu" sheetId="10" r:id="rId13"/>
+    <sheet name="lui" sheetId="19" r:id="rId11"/>
+    <sheet name="mux" sheetId="4" r:id="rId12"/>
+    <sheet name="cu" sheetId="5" r:id="rId13"/>
+    <sheet name="Alu" sheetId="10" r:id="rId14"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="294">
   <si>
     <t>阶段</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -852,6 +853,15 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>GPR.WREG</t>
+  </si>
+  <si>
+    <t>GPR.WDATA</t>
+  </si>
+  <si>
+    <t>WB</t>
+  </si>
+  <si>
     <t>GPR.RREG1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -888,9 +898,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>BLEZ、BGTZ</t>
-  </si>
-  <si>
     <t>MULT、DIVU\</t>
   </si>
   <si>
@@ -980,17 +987,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>LB、LHU\SB、SH、</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SUB、SUBU、SLTI、SLTIU、SLTU、</t>
-  </si>
-  <si>
-    <t>SRL、SRA、SLLV、LUI、</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>beq</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1064,6 +1060,26 @@
   </si>
   <si>
     <t>6'b001100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>010100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6'b100100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>imm 0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6'b010100</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1083,23 +1099,102 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>010100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>100100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6'b100100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6'b010100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>imm 0</t>
+    <t>6'b000100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sub</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6'b000101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sltu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IR.OUT[20:16]</t>
+  </si>
+  <si>
+    <t>WB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IR.OUT[15:0] + 0^15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ir.out[15:0]+0^15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lsgnextent.out</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SRL、SRA、SLLV、</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>算术右移</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>011000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>逻辑右移</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>101000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>逻辑左移</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>110000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6'b011000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6'b101000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6'b110000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sra</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>srl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sll</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6'b011000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6'b101000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sra/srl/sll::ir.out[10:6]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1164,7 +1259,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1174,6 +1269,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1257,7 +1358,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyFill="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1285,6 +1386,13 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1603,8 +1711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:E29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2000,21 +2108,21 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="23.77734375" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -2023,7 +2131,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -2143,9 +2251,8 @@
         <v>79</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="D11" s="1"/>
+        <v>236</v>
+      </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5">
@@ -2192,25 +2299,27 @@
         <v>32</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="1"/>
+      <c r="D15" s="1" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="10" t="s">
         <v>169</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>38</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -2218,13 +2327,13 @@
         <v>169</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>38</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -2232,13 +2341,13 @@
         <v>169</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>223</v>
+        <v>271</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>38</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>230</v>
+        <v>272</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -2246,7 +2355,7 @@
         <v>169</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>179</v>
+        <v>224</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>38</v>
@@ -2256,66 +2365,111 @@
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="1" t="s">
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="C21" s="1" t="s">
+      <c r="B26" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="1" t="s">
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="1"/>
@@ -2334,6 +2488,31 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2347,10 +2526,165 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2425,6 +2759,12 @@
       <c r="D4" t="s">
         <v>121</v>
       </c>
+      <c r="E4" t="s">
+        <v>277</v>
+      </c>
+      <c r="F4" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
@@ -2451,7 +2791,7 @@
         <v>127</v>
       </c>
       <c r="D6" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="E6" t="s">
         <v>128</v>
@@ -2493,16 +2833,16 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B9" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="C9" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="D9" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -2511,12 +2851,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2581,7 +2921,7 @@
         <v>145</v>
       </c>
       <c r="C3" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="D3" t="s">
         <v>145</v>
@@ -2604,7 +2944,7 @@
         <v>145</v>
       </c>
       <c r="C4" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="D4" t="s">
         <v>151</v>
@@ -2656,7 +2996,7 @@
         <v>146</v>
       </c>
       <c r="G6" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="H6" t="s">
         <v>183</v>
@@ -2709,12 +3049,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2792,7 +3132,7 @@
         <v>194</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15" thickBot="1">
@@ -2816,47 +3156,47 @@
         <v>197</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="6" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="6" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="12.6" customHeight="1">
       <c r="A16" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15" thickBot="1">
@@ -2864,32 +3204,41 @@
         <v>194</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>243</v>
+      <c r="A19" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>242</v>
+      <c r="A20" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
-        <v>218</v>
+      <c r="A21" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -2903,7 +3252,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:D24"/>
+      <selection activeCell="C24" sqref="A23:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3224,13 +3573,13 @@
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="12" t="s">
         <v>52</v>
       </c>
       <c r="D23" s="1"/>
@@ -3268,7 +3617,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="A23" sqref="A23:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3592,13 +3941,13 @@
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="12" t="s">
         <v>101</v>
       </c>
       <c r="D23" s="1"/>
@@ -3626,7 +3975,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection sqref="A1:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3991,7 +4340,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -4040,7 +4389,7 @@
         <v>32</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>38</v>
@@ -4166,7 +4515,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:C14"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4302,7 +4651,7 @@
         <v>163</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -4325,7 +4674,7 @@
         <v>109</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>52</v>
@@ -4549,7 +4898,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -4588,7 +4937,7 @@
         <v>163</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -4611,7 +4960,7 @@
         <v>32</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>38</v>
@@ -4650,7 +4999,7 @@
         <v>109</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>52</v>
@@ -4746,8 +5095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4876,13 +5225,13 @@
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="12" t="s">
         <v>22</v>
       </c>
       <c r="D11" s="1"/>
@@ -4974,13 +5323,13 @@
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="12" t="s">
         <v>28</v>
       </c>
       <c r="D19" s="1"/>
@@ -5026,13 +5375,13 @@
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="12" t="s">
         <v>36</v>
       </c>
       <c r="D23" s="1"/>
@@ -5042,13 +5391,13 @@
         <v>169</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>38</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -5056,13 +5405,13 @@
         <v>169</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>38</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E25" s="1"/>
     </row>
@@ -5071,13 +5420,13 @@
         <v>169</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>38</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E26" s="1"/>
     </row>
@@ -5086,13 +5435,13 @@
         <v>169</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="C27" s="10" t="s">
         <v>38</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E27" s="1"/>
     </row>
@@ -5101,13 +5450,13 @@
         <v>169</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>38</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -5115,13 +5464,13 @@
         <v>169</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>38</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -5213,10 +5562,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D27" sqref="A25:D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5227,7 +5576,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -5236,7 +5585,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -5431,13 +5780,13 @@
         <v>169</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>38</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -5445,28 +5794,27 @@
         <v>169</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>221</v>
+        <v>269</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>38</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>228</v>
-      </c>
-      <c r="E18" s="1"/>
+        <v>270</v>
+      </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="10" t="s">
         <v>169</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>38</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E19" s="1"/>
     </row>
@@ -5475,13 +5823,13 @@
         <v>169</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>223</v>
+        <v>271</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>38</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>230</v>
+        <v>272</v>
       </c>
       <c r="E20" s="1"/>
     </row>
@@ -5490,7 +5838,7 @@
         <v>169</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>179</v>
+        <v>224</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>38</v>
@@ -5498,13 +5846,14 @@
       <c r="D21" s="10" t="s">
         <v>231</v>
       </c>
+      <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="10" t="s">
         <v>169</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>38</v>
@@ -5512,64 +5861,110 @@
       <c r="D22" s="10" t="s">
         <v>232</v>
       </c>
+      <c r="E22" s="1"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="1" t="s">
+    <row r="29" spans="1:5">
+      <c r="A29" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="C24" s="1" t="s">
+      <c r="B29" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="B25" s="1" t="s">
+    <row r="30" spans="1:5">
+      <c r="A30" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="1"/>
@@ -5593,6 +5988,31 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>